<commit_message>
added data provider code
</commit_message>
<xml_diff>
--- a/uiAutomation/src/main/java/testData/TestData.xlsx
+++ b/uiAutomation/src/main/java/testData/TestData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hybridFramework\uiAutomation\src\main\java\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13065" windowHeight="3075" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="3330"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
     <sheet name="Browser&amp;URL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A7:I14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -385,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding changes in pom to execute pom from jenkins
</commit_message>
<xml_diff>
--- a/uiAutomation/src/main/java/testData/TestData.xlsx
+++ b/uiAutomation/src/main/java/testData/TestData.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hybridFramework\uiAutomation\src\main\java\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="3330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12525" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
     <sheet name="Browser&amp;URL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A7:I14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,25 +36,25 @@
     <t>RunMode</t>
   </si>
   <si>
+    <t>erp@admin</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Browser</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>http://52.172.14.165/JNVURESULT</t>
+  </si>
+  <si>
+    <t>Chrome</t>
+  </si>
+  <si>
     <t>Jnvu@)!^</t>
-  </si>
-  <si>
-    <t>erp@admin</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Browser</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>http://52.172.14.165/JNVURESULT</t>
-  </si>
-  <si>
-    <t>Chrome</t>
   </si>
 </sst>
 </file>
@@ -382,7 +386,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,13 +409,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -438,18 +442,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final frame work code
</commit_message>
<xml_diff>
--- a/uiAutomation/src/main/java/testData/TestData.xlsx
+++ b/uiAutomation/src/main/java/testData/TestData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hybridFramework\uiAutomation\src\main\java\testData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12525" windowHeight="6450"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14475" windowHeight="3240"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
     <sheet name="Browser&amp;URL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:L8"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>

</xml_diff>